<commit_message>
0670 0680 + betere foutmelding label missing
</commit_message>
<xml_diff>
--- a/0.98-3-Validatie-_en_conformiteitsregels_TPOD/documenten/Validatie-en-Conformiteitsregels Totaal v0.9 - incl onderscheidOntwerpDefinitief.xlsx
+++ b/0.98-3-Validatie-_en_conformiteitsregels_TPOD/documenten/Validatie-en-Conformiteitsregels Totaal v0.9 - incl onderscheidOntwerpDefinitief.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_schematron\0.98-3-Validatie-_en_conformiteitsregels_TPOD\documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D91DB24-56D4-4E7C-8964-A5F26C80FD4A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47E71B69-184B-46B3-80E4-DB8DF5496587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
   </bookViews>
@@ -29456,8 +29456,8 @@
   <dimension ref="A1:V219"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
+      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -31228,7 +31228,7 @@
       </c>
     </row>
     <row r="27" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1" t="s">
+      <c r="A27" s="31" t="s">
         <v>563</v>
       </c>
       <c r="B27" s="2" t="s">
@@ -31294,7 +31294,7 @@
       </c>
     </row>
     <row r="28" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
+      <c r="A28" s="31" t="s">
         <v>564</v>
       </c>
       <c r="B28" s="2" t="s">
@@ -31360,7 +31360,7 @@
       </c>
     </row>
     <row r="29" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
+      <c r="A29" s="31" t="s">
         <v>540</v>
       </c>
       <c r="B29" s="2" t="s">
@@ -31428,7 +31428,7 @@
       </c>
     </row>
     <row r="30" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
+      <c r="A30" s="31" t="s">
         <v>541</v>
       </c>
       <c r="B30" s="2" t="s">

</xml_diff>

<commit_message>
controle op toepassing van validatie
</commit_message>
<xml_diff>
--- a/0.98-3-Validatie-_en_conformiteitsregels_TPOD/documenten/Validatie-en-Conformiteitsregels Totaal v0.9 - incl onderscheidOntwerpDefinitief.xlsx
+++ b/0.98-3-Validatie-_en_conformiteitsregels_TPOD/documenten/Validatie-en-Conformiteitsregels Totaal v0.9 - incl onderscheidOntwerpDefinitief.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_schematron\0.98-3-Validatie-_en_conformiteitsregels_TPOD\documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D790B272-0BD3-4B52-B011-52B2028141B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61C81AB-8B39-4D19-8C0D-B021BC14C1F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
+    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
   </bookViews>
   <sheets>
     <sheet name="TotaalOverzicht" sheetId="6" r:id="rId1"/>
@@ -2178,7 +2178,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2200,6 +2200,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2264,7 +2270,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2385,6 +2391,9 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2400,8 +2409,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -29542,17 +29551,19 @@
   <dimension ref="A1:V217"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A107" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A114" sqref="A114"/>
+      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A115" sqref="A115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.77734375" customWidth="1"/>
-    <col min="2" max="2" width="83" customWidth="1"/>
+    <col min="2" max="2" width="12.21875" customWidth="1"/>
     <col min="3" max="4" width="10.77734375" customWidth="1"/>
-    <col min="5" max="5" width="20.77734375" customWidth="1"/>
-    <col min="6" max="8" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="8.21875" customWidth="1"/>
+    <col min="6" max="6" width="12.77734375" customWidth="1"/>
+    <col min="7" max="7" width="4.5546875" customWidth="1"/>
+    <col min="8" max="8" width="3.6640625" customWidth="1"/>
     <col min="9" max="15" width="9.33203125" style="20" customWidth="1"/>
     <col min="16" max="22" width="9.33203125" customWidth="1"/>
   </cols>
@@ -29760,7 +29771,7 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="57" t="s">
         <v>560</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -30502,7 +30513,7 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
+      <c r="A15" s="57" t="s">
         <v>530</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -30840,7 +30851,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="56" t="s">
+      <c r="A20" s="57" t="s">
         <v>534</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -31113,7 +31124,7 @@
       <c r="A24" s="31" t="s">
         <v>537</v>
       </c>
-      <c r="B24" s="50" t="s">
+      <c r="B24" s="51" t="s">
         <v>74</v>
       </c>
       <c r="C24" s="3" t="s">
@@ -31246,7 +31257,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="56" t="s">
+      <c r="A26" s="57" t="s">
         <v>539</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -31582,7 +31593,7 @@
       </c>
     </row>
     <row r="31" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="57" t="s">
         <v>542</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -31918,7 +31929,7 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="56" t="s">
+      <c r="A36" s="57" t="s">
         <v>545</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -32322,7 +32333,7 @@
       </c>
     </row>
     <row r="42" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="56" t="s">
+      <c r="A42" s="57" t="s">
         <v>549</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -33330,7 +33341,7 @@
       </c>
     </row>
     <row r="57" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="1" t="s">
+      <c r="A57" s="31" t="s">
         <v>558</v>
       </c>
       <c r="B57" s="2" t="s">
@@ -35740,7 +35751,7 @@
       </c>
     </row>
     <row r="93" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="1" t="s">
+      <c r="A93" s="31" t="s">
         <v>45</v>
       </c>
       <c r="B93" s="9" t="s">
@@ -35876,7 +35887,7 @@
       </c>
     </row>
     <row r="95" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A95" s="31" t="s">
+      <c r="A95" s="50" t="s">
         <v>121</v>
       </c>
       <c r="B95" s="2" t="s">
@@ -36080,7 +36091,7 @@
       </c>
     </row>
     <row r="98" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="55" t="s">
+      <c r="A98" s="56" t="s">
         <v>137</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -36148,7 +36159,7 @@
       </c>
     </row>
     <row r="99" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="56" t="s">
+      <c r="A99" s="57" t="s">
         <v>137</v>
       </c>
       <c r="B99" s="2" t="s">
@@ -36828,10 +36839,10 @@
       </c>
     </row>
     <row r="109" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="51" t="s">
+      <c r="A109" s="52" t="s">
         <v>641</v>
       </c>
-      <c r="B109" s="52" t="s">
+      <c r="B109" s="53" t="s">
         <v>642</v>
       </c>
       <c r="C109" s="3" t="s">
@@ -36896,10 +36907,10 @@
       </c>
     </row>
     <row r="110" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A110" s="57" t="s">
+      <c r="A110" s="58" t="s">
         <v>667</v>
       </c>
-      <c r="B110" s="53" t="s">
+      <c r="B110" s="54" t="s">
         <v>662</v>
       </c>
       <c r="C110" s="32" t="s">
@@ -36964,7 +36975,7 @@
       </c>
     </row>
     <row r="111" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A111" s="58" t="s">
+      <c r="A111" s="59" t="s">
         <v>661</v>
       </c>
       <c r="B111" s="36" t="s">
@@ -37032,7 +37043,7 @@
       </c>
     </row>
     <row r="112" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="58" t="s">
+      <c r="A112" s="59" t="s">
         <v>668</v>
       </c>
       <c r="B112" s="36" t="s">
@@ -37100,7 +37111,7 @@
       </c>
     </row>
     <row r="113" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A113" s="58" t="s">
+      <c r="A113" s="59" t="s">
         <v>669</v>
       </c>
       <c r="B113" s="36" t="s">
@@ -37168,7 +37179,7 @@
       </c>
     </row>
     <row r="114" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A114" s="58" t="s">
+      <c r="A114" s="59" t="s">
         <v>670</v>
       </c>
       <c r="B114" s="36" t="s">
@@ -37236,10 +37247,10 @@
       </c>
     </row>
     <row r="115" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A115" s="39" t="s">
+      <c r="A115" s="31" t="s">
         <v>671</v>
       </c>
-      <c r="B115" s="54" t="s">
+      <c r="B115" s="55" t="s">
         <v>660</v>
       </c>
       <c r="C115" s="32" t="s">

</xml_diff>

<commit_message>
aanpassingen validatie- en conformiteitsregels
</commit_message>
<xml_diff>
--- a/0.98-3-Validatie-_en_conformiteitsregels_TPOD/documenten/Validatie-en-Conformiteitsregels Totaal v0.9 - incl onderscheidOntwerpDefinitief.xlsx
+++ b/0.98-3-Validatie-_en_conformiteitsregels_TPOD/documenten/Validatie-en-Conformiteitsregels Totaal v0.9 - incl onderscheidOntwerpDefinitief.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Default.DESKTOP-NDDI22K\Documents\Geonovum\github\xml_schematron\0.98-3-Validatie-_en_conformiteitsregels_TPOD\documenten\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\RicharddeGraaf\Desktop\Geonovum\4 - Voorbeeldbestanden\GITHub\xml_schematron\0.98-3-Validatie-_en_conformiteitsregels_TPOD\documenten\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C61C81AB-8B39-4D19-8C0D-B021BC14C1F2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74E1BF25-6B18-4A91-B580-ED742E13826B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="348" windowWidth="23256" windowHeight="12720" activeTab="2" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{CAF58E0D-33FE-46EB-ADA3-90D1B902B379}"/>
   </bookViews>
   <sheets>
     <sheet name="TotaalOverzicht" sheetId="6" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13874" uniqueCount="672">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13918" uniqueCount="677">
   <si>
     <t>ID</t>
   </si>
@@ -2104,12 +2104,56 @@
   <si>
     <t>TPOD2050</t>
   </si>
+  <si>
+    <t>Ieder OwObject heeft minstens een OwObject dat ernaar verwijst.</t>
+  </si>
+  <si>
+    <t>TPOD2060</t>
+  </si>
+  <si>
+    <t>TPOD2070</t>
+  </si>
+  <si>
+    <t>Als een verwijzing naar een Lid is gemaakt mag er geen verwijzing meer gemaakt worden naar het artikel dat boven dit Lid hangt. (RegeltekstID alleen op Lid-niveau of alleen op Artikel-niveau.)</t>
+  </si>
+  <si>
+    <r>
+      <t>Als de activiteit een bepaalde regeltekstID heeft dan moet deze overeenkomen met de ID die je via de logische relaties vindt (regeltekst naar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> juridische regel (regel voor iedereen) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Wingdings"/>
+        <charset val="2"/>
+      </rPr>
+      <t>naar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> activiteitaanduiding).</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -2177,8 +2221,20 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Wingdings"/>
+      <charset val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2212,6 +2268,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2397,9 +2459,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2417,6 +2476,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -29550,9 +29612,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511BE904-3D15-4F6E-B5B9-2AD212EB1E09}">
   <dimension ref="A1:V217"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A98" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A115" sqref="A115"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A100" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -29771,7 +29833,7 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="56" t="s">
         <v>560</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -30513,7 +30575,7 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
+      <c r="A15" s="56" t="s">
         <v>530</v>
       </c>
       <c r="B15" s="2" t="s">
@@ -30851,7 +30913,7 @@
       </c>
     </row>
     <row r="20" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="57" t="s">
+      <c r="A20" s="56" t="s">
         <v>534</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -31257,7 +31319,7 @@
       </c>
     </row>
     <row r="26" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="57" t="s">
+      <c r="A26" s="56" t="s">
         <v>539</v>
       </c>
       <c r="B26" s="2" t="s">
@@ -31593,7 +31655,7 @@
       </c>
     </row>
     <row r="31" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="57" t="s">
+      <c r="A31" s="56" t="s">
         <v>542</v>
       </c>
       <c r="B31" s="2" t="s">
@@ -31929,7 +31991,7 @@
       </c>
     </row>
     <row r="36" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="57" t="s">
+      <c r="A36" s="56" t="s">
         <v>545</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -32333,7 +32395,7 @@
       </c>
     </row>
     <row r="42" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="57" t="s">
+      <c r="A42" s="56" t="s">
         <v>549</v>
       </c>
       <c r="B42" s="2" t="s">
@@ -36091,7 +36153,7 @@
       </c>
     </row>
     <row r="98" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="56" t="s">
+      <c r="A98" s="55" t="s">
         <v>137</v>
       </c>
       <c r="B98" s="3" t="s">
@@ -36159,7 +36221,7 @@
       </c>
     </row>
     <row r="99" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="57" t="s">
+      <c r="A99" s="56" t="s">
         <v>137</v>
       </c>
       <c r="B99" s="2" t="s">
@@ -36839,11 +36901,11 @@
       </c>
     </row>
     <row r="109" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A109" s="52" t="s">
+      <c r="A109" s="59" t="s">
         <v>641</v>
       </c>
-      <c r="B109" s="53" t="s">
-        <v>642</v>
+      <c r="B109" s="52" t="s">
+        <v>672</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>123</v>
@@ -36907,10 +36969,10 @@
       </c>
     </row>
     <row r="110" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A110" s="58" t="s">
+      <c r="A110" s="57" t="s">
         <v>667</v>
       </c>
-      <c r="B110" s="54" t="s">
+      <c r="B110" s="53" t="s">
         <v>662</v>
       </c>
       <c r="C110" s="32" t="s">
@@ -36975,7 +37037,7 @@
       </c>
     </row>
     <row r="111" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A111" s="59" t="s">
+      <c r="A111" s="58" t="s">
         <v>661</v>
       </c>
       <c r="B111" s="36" t="s">
@@ -37043,7 +37105,7 @@
       </c>
     </row>
     <row r="112" spans="1:22" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A112" s="59" t="s">
+      <c r="A112" s="58" t="s">
         <v>668</v>
       </c>
       <c r="B112" s="36" t="s">
@@ -37111,7 +37173,7 @@
       </c>
     </row>
     <row r="113" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A113" s="59" t="s">
+      <c r="A113" s="58" t="s">
         <v>669</v>
       </c>
       <c r="B113" s="36" t="s">
@@ -37179,7 +37241,7 @@
       </c>
     </row>
     <row r="114" spans="1:22" ht="13.8" x14ac:dyDescent="0.3">
-      <c r="A114" s="59" t="s">
+      <c r="A114" s="58" t="s">
         <v>670</v>
       </c>
       <c r="B114" s="36" t="s">
@@ -37250,7 +37312,7 @@
       <c r="A115" s="31" t="s">
         <v>671</v>
       </c>
-      <c r="B115" s="55" t="s">
+      <c r="B115" s="54" t="s">
         <v>660</v>
       </c>
       <c r="C115" s="32" t="s">
@@ -37314,11 +37376,141 @@
         <v>134</v>
       </c>
     </row>
-    <row r="116" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A116" s="45"/>
-    </row>
-    <row r="117" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
-      <c r="A117" s="45"/>
+    <row r="116" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A116" s="1" t="s">
+        <v>673</v>
+      </c>
+      <c r="B116" s="54" t="s">
+        <v>675</v>
+      </c>
+      <c r="C116" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E116" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F116" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="I116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="J116" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="K116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="L116" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="M116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="N116" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="O116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="P116" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="R116" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="T116" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="U116" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="V116" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="117" spans="1:22" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A117" s="1" t="s">
+        <v>674</v>
+      </c>
+      <c r="B117" s="54" t="s">
+        <v>676</v>
+      </c>
+      <c r="C117" s="32" t="s">
+        <v>123</v>
+      </c>
+      <c r="D117" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E117" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F117" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="G117" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="H117" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="I117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="J117" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="K117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="L117" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="M117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="N117" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="O117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="P117" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="R117" s="19" t="s">
+        <v>134</v>
+      </c>
+      <c r="S117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="T117" s="18" t="s">
+        <v>134</v>
+      </c>
+      <c r="U117" s="38" t="s">
+        <v>134</v>
+      </c>
+      <c r="V117" s="19" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="118" spans="1:22" ht="13.8" x14ac:dyDescent="0.25">
       <c r="A118" s="45"/>

</xml_diff>